<commit_message>
update 20251124 -- Refactor PPV Tools
</commit_message>
<xml_diff>
--- a/S2T/BASELINE/DebugFramework/PPV/MCChecker/GNR/##Name##_##w##_##LABEL##_PPV_Data.xlsx
+++ b/S2T/BASELINE/DebugFramework/PPV/MCChecker/GNR/##Name##_##w##_##LABEL##_PPV_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Automation\PPV\MCChecker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Automation\Automation\PPV\MCChecker\GNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF690A8-F75B-45E5-AECC-E5CE1EC3A4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C89699-3731-466F-B393-2D5FF3213F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B6A3F570-C7B8-40A8-89EA-A952D4B6B916}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B6A3F570-C7B8-40A8-89EA-A952D4B6B916}"/>
   </bookViews>
   <sheets>
     <sheet name="CHA" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>VisualId</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>BinDesc</t>
+  </si>
+  <si>
+    <t>Program</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -199,11 +202,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -211,11 +225,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -475,7 +535,7 @@
     <tableColumn id="8" xr3:uid="{F7120CC3-0273-43DD-B433-AA977B23897A}" name="Operation"/>
     <tableColumn id="9" xr3:uid="{469AA545-A454-4036-8CA3-85DB9744289F}" name="TestNameNumber"/>
     <tableColumn id="10" xr3:uid="{F4486BB9-8EBB-4796-A792-020AEBC73AB2}" name="TestNameWithoutNumeric"/>
-    <tableColumn id="11" xr3:uid="{3E29E89A-4EB3-4D6E-BC38-F103C02C26E7}" name="PPVRun_MC" dataDxfId="13">
+    <tableColumn id="11" xr3:uid="{3E29E89A-4EB3-4D6E-BC38-F103C02C26E7}" name="PPVRun_MC" dataDxfId="15">
       <calculatedColumnFormula>IF(cha_mc[[#This Row],[TestValue]]&lt;&gt;"0X20000000000000",cha_mc[[#This Row],[LotsSeqKey]]&amp;"-"&amp;cha_mc[[#This Row],[UnitTestingSeqKey]],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -497,24 +557,26 @@
     <tableColumn id="8" xr3:uid="{BD64BBFC-FE97-4702-B4AC-F11C70B0E9B1}" name="Operation"/>
     <tableColumn id="9" xr3:uid="{23B54051-2A23-4C4D-958C-72ABED739074}" name="TestNameNumber"/>
     <tableColumn id="10" xr3:uid="{BFC4E21F-EF8B-413D-A1E2-8FA817E6F4AF}" name="TestNameWithoutNumeric"/>
-    <tableColumn id="12" xr3:uid="{523F8EFA-ED88-411B-A36A-3969625F6763}" name="PPVRun_MC" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{523F8EFA-ED88-411B-A36A-3969625F6763}" name="PPVRun_MC" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F70154BC-6B14-4ED2-9597-E2E503E21502}" name="ppv" displayName="ppv" ref="A1:H2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:H2" xr:uid="{F70154BC-6B14-4ED2-9597-E2E503E21502}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E99145A2-32F3-4EE2-B709-273D9F43015B}" name="VisualId" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{10783810-8563-452A-A516-E986B4A18B86}" name="DpmBucket" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{4C23BF57-63ED-42CF-A065-A56932CFC945}" name="DecimaSite" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{C4845B0C-9AD8-489F-9E5C-3258831D5FAC}" name="DecimaWW" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{DE045528-99BA-4189-B772-1659FCA755D6}" name="DecimaBucket" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{C42F3BF6-0E70-4FEC-8DC5-C5C92CD67CE9}" name="DpmBucketAccuracy" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{EB173296-6B6E-4C4D-9492-E2D75C99B2EA}" name="ProductConfigurationName" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{7536F8C6-1E57-4CA7-8FF9-95F54A9AA415}" name="BinDesc" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F70154BC-6B14-4ED2-9597-E2E503E21502}" name="ppv" displayName="ppv" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="A1:J2" xr:uid="{F70154BC-6B14-4ED2-9597-E2E503E21502}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{E99145A2-32F3-4EE2-B709-273D9F43015B}" name="VisualId" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{10783810-8563-452A-A516-E986B4A18B86}" name="DpmBucket" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4C23BF57-63ED-42CF-A065-A56932CFC945}" name="DecimaSite" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C4845B0C-9AD8-489F-9E5C-3258831D5FAC}" name="DecimaWW" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{DE045528-99BA-4189-B772-1659FCA755D6}" name="DecimaBucket" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{C42F3BF6-0E70-4FEC-8DC5-C5C92CD67CE9}" name="DpmBucketAccuracy" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{EB173296-6B6E-4C4D-9492-E2D75C99B2EA}" name="ProductConfigurationName" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{7536F8C6-1E57-4CA7-8FF9-95F54A9AA415}" name="BinDesc" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{AA40D048-8AF7-4BC6-87C5-536640D7E953}" name="Program" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{5388B4B5-0F96-4125-8B45-14A72C9BCBE5}" name="Lot" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -956,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD37023-CAE0-4F26-B81B-25451DE87D41}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,7 +1035,7 @@
     <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -998,8 +1060,14 @@
       <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1008,6 +1076,8 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>